<commit_message>
# Agregue los graficos de Costos, QC y Burndown Chart para entrega del 27/09
</commit_message>
<xml_diff>
--- a/meetings/BurndownChart.20100927.xlsx
+++ b/meetings/BurndownChart.20100927.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="270" windowWidth="23295" windowHeight="10680"/>
+    <workbookView xWindow="840" yWindow="270" windowWidth="23295" windowHeight="10680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
-    <t>title</t>
-  </si>
-  <si>
-    <t>Crear el diseÃ±o general de la master page del sistema SelfManagement</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de ABM de CampaÃ±as para los Jefes de Cuentas</t>
-  </si>
-  <si>
-    <t>Crear el mockup de la pagina de estadisticas globales de las CampaÃ±as para los Jefes de Cuentas (utilizando un dashboard y soportando busquedas)</t>
-  </si>
-  <si>
     <t>Crear el mockup de la pagina de las estadisticas globales de un Supervisor para los Jefe de Cuentas y Supervisores (utilizando un dashboard)</t>
   </si>
   <si>
@@ -45,24 +33,9 @@
     <t>Crear la estructura inicial de la solucion SelfManagent con todos los proyectos requeridos</t>
   </si>
   <si>
-    <t>DiseÃ±ar el esquema de la base de datos para el sistema SelfManagement</t>
-  </si>
-  <si>
-    <t>Implementar la pantalla de alta de campaÃ±as para el sistema SelfManagement</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>completed</t>
   </si>
   <si>
-    <t>remaining</t>
-  </si>
-  <si>
     <t>Crear VPC con ambiente de desarrollo</t>
   </si>
   <si>
@@ -70,6 +43,33 @@
   </si>
   <si>
     <t>Fecha</t>
+  </si>
+  <si>
+    <t>Crear el diseño general de la master page del sistema SelfManagement</t>
+  </si>
+  <si>
+    <t>Crear el mockup de la pagina de ABM de Campañas para los Jefes de Cuentas</t>
+  </si>
+  <si>
+    <t>Crear el mockup de la pagina de estadisticas globales de las Campañas para los Jefes de Cuentas (utilizando un dashboard y soportando busquedas)</t>
+  </si>
+  <si>
+    <t>Diseñar el esquema de la base de datos para el sistema SelfManagement</t>
+  </si>
+  <si>
+    <t>Implementar la pantalla de alta de campañas para el sistema SelfManagement</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Remaining</t>
   </si>
 </sst>
 </file>
@@ -206,10 +206,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>17</c:v>
@@ -255,11 +255,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90351104"/>
-        <c:axId val="90352640"/>
+        <c:axId val="89433600"/>
+        <c:axId val="89435136"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="90351104"/>
+        <c:axId val="89433600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -267,13 +267,13 @@
         <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90352640"/>
+        <c:crossAx val="89435136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="90352640"/>
+        <c:axId val="89435136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +300,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90351104"/>
+        <c:crossAx val="89433600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -309,7 +309,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -354,10 +354,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:D12" totalsRowShown="0">
   <autoFilter ref="A1:D12"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="title"/>
-    <tableColumn id="2" name="weight"/>
-    <tableColumn id="3" name="status"/>
-    <tableColumn id="4" name="remaining">
+    <tableColumn id="1" name="Title"/>
+    <tableColumn id="2" name="Weight"/>
+    <tableColumn id="3" name="Status"/>
+    <tableColumn id="4" name="Remaining">
       <calculatedColumnFormula>D1-B1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -677,27 +677,27 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <f>SUM(B2:B12)</f>
@@ -707,13 +707,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <f>D2-B2</f>
@@ -723,13 +723,13 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <f t="shared" ref="D4:D12" si="0">D3-B3</f>
@@ -739,13 +739,13 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
@@ -755,13 +755,13 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
@@ -770,13 +770,13 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
@@ -785,13 +785,13 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
@@ -800,13 +800,13 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
@@ -815,13 +815,13 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
@@ -830,13 +830,13 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
@@ -845,13 +845,13 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12">
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -882,10 +882,10 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -893,7 +893,7 @@
         <v>40434</v>
       </c>
       <c r="B2">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -901,7 +901,7 @@
         <v>40435</v>
       </c>
       <c r="B3">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2">

</xml_diff>